<commit_message>
fixed all Excel_Ini files for the new format
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/GuildName.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/GuildName.xlsx
@@ -1,18 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
-    <sheet name="Property" sheetId="1" r:id="rId1"/>
+    <sheet name="Property1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -22,12 +17,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>GuildID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>工会ID</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -35,27 +67,370 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -63,31 +438,327 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFD7D7D7"/>
         </patternFill>
       </fill>
@@ -98,26 +769,16 @@
         <i val="0"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
+        <patternFill patternType="none"/>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
+    <tableStyle name="MySqlDefault" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -167,71 +828,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -449,16 +1110,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="8.25" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
@@ -469,18 +1131,70 @@
     <col min="10" max="10" width="81" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B1" s="1"/>
+    <row r="1" s="1" customFormat="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F6 F7:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>